<commit_message>
Fixed night time data processing logic and implemented level 1
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Magh" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -526,9 +526,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>489960</xdr:colOff>
+      <xdr:colOff>489600</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -542,7 +542,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="99360" y="79200"/>
-          <a:ext cx="1245960" cy="373320"/>
+          <a:ext cx="1245600" cy="372960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -737,7 +737,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="W22" activeCellId="0" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed small format change
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\overtime-app-nac\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78318127-E672-45C3-9886-904813E9806A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AED2B3-3FDA-4E98-8CE9-865A7F6C0590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,15 +239,6 @@
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -328,7 +319,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -440,8 +431,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="46" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -449,34 +439,10 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -486,6 +452,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -732,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:WVT49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,21 +1413,21 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="60" t="s">
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="63" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1445,27 +1435,27 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61" t="s">
+      <c r="E8" s="64"/>
+      <c r="F8" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="61"/>
+      <c r="G8" s="64"/>
       <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="61" t="s">
+      <c r="I8" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="60"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="63"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
@@ -1710,68 +1700,68 @@
       <c r="L22" s="29"/>
     </row>
     <row r="23" spans="1:12" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="62">
+      <c r="A23" s="53">
         <v>14</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="64"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="55"/>
     </row>
     <row r="24" spans="1:12" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="62">
+      <c r="A24" s="53">
         <v>15</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="64"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="55"/>
     </row>
     <row r="25" spans="1:12" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="62">
+      <c r="A25" s="53">
         <v>16</v>
       </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="63"/>
-      <c r="L25" s="65"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="56"/>
     </row>
     <row r="26" spans="1:12" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="62">
+      <c r="A26" s="53">
         <v>17</v>
       </c>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="63"/>
-      <c r="L26" s="63"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="28">
@@ -2040,11 +2030,11 @@
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="50" t="s">
+      <c r="I43" s="48"/>
+      <c r="J43" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="K43" s="51" t="s">
+      <c r="K43" s="50" t="s">
         <v>23</v>
       </c>
       <c r="L43" s="8"/>
@@ -2055,13 +2045,13 @@
       </c>
       <c r="B44" s="45"/>
       <c r="C44" s="46"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="15"/>
-      <c r="F44" s="48" t="s">
+      <c r="F44" s="47" t="s">
         <v>31</v>
       </c>
       <c r="G44" s="44"/>
-      <c r="H44" s="53"/>
+      <c r="H44" s="52"/>
       <c r="I44" s="37"/>
       <c r="J44" s="37"/>
       <c r="K44" s="37"/>
@@ -2647,26 +2637,26 @@
       <c r="K45" s="36"/>
     </row>
     <row r="46" spans="1:780 1028:1804 2052:2828 3076:3852 4100:4876 5124:5900 6148:6924 7172:7948 8196:8972 9220:9996 10244:11020 11268:12044 12292:13068 13316:14092 14340:15116 15364:16140" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B46" s="54"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="38"/>
-      <c r="D46" s="55" t="s">
+      <c r="D46" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
       <c r="G46" s="38"/>
-      <c r="H46" s="56" t="s">
+      <c r="H46" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="57" t="s">
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="L46" s="57"/>
+      <c r="L46" s="60"/>
     </row>
     <row r="47" spans="1:780 1028:1804 2052:2828 3076:3852 4100:4876 5124:5900 6148:6924 7172:7948 8196:8972 9220:9996 10244:11020 11268:12044 12292:13068 13316:14092 14340:15116 15364:16140" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="38"/>

</xml_diff>

<commit_message>
Fixed mistake in template
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\overtime-app-nac\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AED2B3-3FDA-4E98-8CE9-865A7F6C0590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3A72A0-A4AE-4292-93A1-0E45994CB6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>After 23:30</t>
   </si>
   <si>
-    <t>Total Hours:</t>
-  </si>
-  <si>
     <t>Prepared by:</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Dashain Hours:</t>
+  </si>
+  <si>
+    <t>Total Regular Hours:</t>
   </si>
 </sst>
 </file>
@@ -151,7 +151,7 @@
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +259,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -319,7 +326,7 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -477,6 +484,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="46" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -722,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:WVT49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,15 +2048,15 @@
       <c r="L43" s="8"/>
     </row>
     <row r="44" spans="1:780 1028:1804 2052:2828 3076:3852 4100:4876 5124:5900 6148:6924 7172:7948 8196:8972 9220:9996 10244:11020 11268:12044 12292:13068 13316:14092 14340:15116 15364:16140" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47" t="s">
-        <v>26</v>
+      <c r="A44" s="65" t="s">
+        <v>31</v>
       </c>
       <c r="B44" s="45"/>
       <c r="C44" s="46"/>
       <c r="D44" s="51"/>
       <c r="E44" s="15"/>
       <c r="F44" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G44" s="44"/>
       <c r="H44" s="52"/>
@@ -2638,23 +2646,23 @@
     </row>
     <row r="46" spans="1:780 1028:1804 2052:2828 3076:3852 4100:4876 5124:5900 6148:6924 7172:7948 8196:8972 9220:9996 10244:11020 11268:12044 12292:13068 13316:14092 14340:15116 15364:16140" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="57"/>
       <c r="C46" s="38"/>
       <c r="D46" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E46" s="58"/>
       <c r="F46" s="58"/>
       <c r="G46" s="38"/>
       <c r="H46" s="59" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I46" s="59"/>
       <c r="J46" s="59"/>
       <c r="K46" s="60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L46" s="60"/>
     </row>

</xml_diff>